<commit_message>
Added excel for eliminate
</commit_message>
<xml_diff>
--- a/src/test/resources/Lists/ListOfRecipes.xlsx
+++ b/src/test/resources/Lists/ListOfRecipes.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="79">
   <si>
     <t>Recipe ID</t>
   </si>
@@ -80,16 +80,227 @@
     <t>Allergies</t>
   </si>
   <si>
+    <t>3554</t>
+  </si>
+  <si>
+    <t>Cabbage Jowar Muthias</t>
+  </si>
+  <si>
+    <t>Snack/Lunch</t>
+  </si>
+  <si>
+    <t>Veg</t>
+  </si>
+  <si>
+    <t>grated cabbage ,
+ jowar (white millet) flour ,
+ low fat curds (dahi) ,
+ chopped coriander (dhania) ,
+ lemon juice ,
+ ginger-green chilli paste ,
+ garlic (lehsun) paste ,
+ turmeric powder (haldi) ,
+ asafoetida (hing) ,
+ salt ,
+ oil ,
+ cumin seeds (jeera) ,
+ curry leaves (kadi patta) ,
+ chopped coriander (dhania) ,
+ green chutney</t>
+  </si>
+  <si>
+    <t>10 mins</t>
+  </si>
+  <si>
+    <t>29 mins</t>
+  </si>
+  <si>
+    <t>To make cabbage jowar muthias, combine the cabbage, jowar flour, curds, coriander, lemon juice, ginger-green chilli paste, garlic paste, turmeric powder, ¼ tsp of asafoetida and salt in a deep bowl and knead into a soft dough using approx. ¼ cup of water.,
+cabbage jowar muthias,
+Divide the dough into 2 equal portions and shape each portion into 125 mm. (5") cylindrical roll.,
+Arrange both the rolls on a greased sieve and steam in a steamer for 20 to 25 minutes. Allow it to cool completely.,
+Once cooled, cut each roll into 13 mm. (½”) thick slices and keep aside.,
+Heat the oil in a broad non-stick pan and add the cumin seeds.,
+When the seeds crackle, add the remaining ¼ tsp of asafoetida and curry leaves and sauté for a few seconds.,
+Add the sliced muthias, mix well and cook on a medium flame for 2 to 3 minutes or till they turn light brown in colour, while tossing gently and occasionally.,
+Garnish the cabbage jowar muthias with coriander and serve hot with green chutney.,
+cabbage jowar muthias</t>
+  </si>
+  <si>
+    <t>Energy: 146 cal,
+ Protein: 4.6 g,
+ Carbohydrates: 26.4 g,
+ Fiber: 4.1 g,
+ Fat: 2.4 g,
+ Cholesterol: 0 mg,
+ Sodium: 16.3 mg</t>
+  </si>
+  <si>
+    <t>Diabetes,
+Hypertension,
+Hypertension</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/cabbage-jowar-muthias-3554r</t>
+  </si>
+  <si>
+    <t>Add</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes: grated cabbage -
+ garlic (lehsun) paste </t>
+  </si>
+  <si>
+    <t>33147</t>
+  </si>
+  <si>
+    <t>Cabbage Jowar Muthias, How To Make Muthia At Home</t>
+  </si>
+  <si>
+    <t>Snacks</t>
+  </si>
+  <si>
+    <t>grated cabbage ,
+ jowar (white millet) flour ,
+ curd (dahi) ,
+ chopped coriander (dhania) ,
+ lemon juice ,
+ ginger-green chilli paste ,
+ garlic (lehsun) paste ,
+ turmeric powder (haldi) ,
+ asafoetida (hing) ,
+ sugar ,
+ salt ,
+ oil ,
+ cumin seeds (jeera) ,
+ curry leaves (kadi patta) ,
+ chopped coriander (dhania)</t>
+  </si>
+  <si>
+    <t>To make cabbage jowar muthias, combine the cabbage, jowar flour, curds, coriander, lemon juice, ginger-green chilli paste, garlic paste, turmeric powder, ¼ tsp of asafoetida, sugar and salt in a deep bowl and knead into a soft dough using approx. ¼ cup of water.,
+cabbage jowar muthias,
+Divide the dough into 2 equal portions and shape each portion into 125 mm. (5") cylindrical roll.,
+Arrange both the rolls on a greased sieve and steam in a steamer for 20 to 25 minutes. Allow it to cool completely.,
+Once cooled, cut each roll into 13 mm. (½”) thick slices and keep aside.,
+Heat the oil in a broad non-stick pan and add the cumin seeds.,
+When the seeds crackle, add the remaining ¼ tsp of asafoetida and curry leaves and sauté for a few seconds.,
+Add the sliced cabbage jowar muthias, mix well and cook on a medium flame for 2 to 3 minutes or till they turn light brown in colour, while tossing gently and occasionally.,
+cabbage jowar muthias,
+Garnish the cabbage jowar muthias with coriander and serve hot with green chutney.,
+cabbage jowar muthias</t>
+  </si>
+  <si>
+    <t>Energy: 347 cal,
+ Protein: 7 g,
+ Carbohydrates: 47.6 g,
+ Fiber: 6.1 g,
+ Fat: 13.7 g,
+ Cholesterol: 4 mg,
+ Sodium: 16.7 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/cabbage-jowar-muthias-how-to-make-muthia-at-home-33147r</t>
+  </si>
+  <si>
+    <t>22358</t>
+  </si>
+  <si>
+    <t>Jowar Pyaz ki Roti, Low Acidity Recipe</t>
+  </si>
+  <si>
+    <t>jowar (white millet) flour ,
+ chopped spring onions whites ,
+ green chilli paste ,
+ oil ,
+ salt ,
+ jowar (white millet) flour ,
+ oil</t>
+  </si>
+  <si>
+    <t>12 mins</t>
+  </si>
+  <si>
+    <t>To make jowar pyaz ki roti, combine all the ingredients in a deep bowl and knead into a soft dough using enough hot water.,
+jowar pyaz ki roti,
+Divide the dough into 4 equal portions and roll each portion into a 150 mm. (6") diameter thick circle using a little jowar flour for rolling.,
+Heat a non-stick tava (griddle) and cook each roti, using ¼ tsp of oil, till brown spots appear on both the sides.,
+Serve the jowar pyaz ki roti immediately.,
+jowar pyaz ki roti</t>
+  </si>
+  <si>
+    <t>Energy: 110 cal,
+ Protein: 2.7 g,
+ Carbohydrates: 18.2 g,
+ Fiber: 2.5 g,
+ Fat: 3 g,
+ Cholesterol: 0 mg,
+ Sodium: 2.1 mg</t>
+  </si>
+  <si>
+    <t>Diabetes,
+Hypothyroidism,
+Hypertension,
+PCOS</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/jowar-pyaz-ki-roti-low-acidity-recipe-22358r</t>
+  </si>
+  <si>
+    <t>42672</t>
+  </si>
+  <si>
+    <t>Jowar and Moong Dal Khichdi</t>
+  </si>
+  <si>
+    <t>Lunch</t>
+  </si>
+  <si>
+    <t>jowar (white millet) ,
+ yellow moong dal (split yellow gram) ,
+ salt ,
+ ghee ,
+ cumin seeds (jeera) ,
+ asafoetida (hing) ,
+ turmeric powder (haldi)</t>
+  </si>
+  <si>
+    <t>2 mins</t>
+  </si>
+  <si>
+    <t>24 mins</t>
+  </si>
+  <si>
+    <t>To make jowar and moong dal khichdi, clean, wash and soak the jowar in enough water in a deep bowl overnight or at least for 10 hours.,
+jowar and moong dal khichdi,
+Next day, drain it and discard the water.,
+Combine the jowar, moong dal, salt and 2 ½ cups of water in a pressure cooker, mix well and pressure cook for 7 whistles.,
+Allow the steam to escape before opening the lid. Keep aside.,
+For the tempering, heat the ghee in a small non-stick pan and add the cumin seeds.,
+When the seeds crackle, add the asafoetida, turmeric powder and sauté for a few seconds.,
+Add the tempering to the khichdi, mix well and cook on a medium flame for 2 to 3 minutes, while stirring occasionally.,
+Serve the jowar and moong dal khichdi immediately.,
+jowar and moong dal khichdi</t>
+  </si>
+  <si>
+    <t>Energy: 160 cal,
+ Protein: 6.8 g,
+ Carbohydrates: 26.3 g,
+ Fiber: 3.5 g,
+ Fat: 3.1 g,
+ Cholesterol: 0 mg,
+ Sodium: 6.7 mg</t>
+  </si>
+  <si>
+    <t>https://www.tarladalal.com/jowar-and-moong-dal-khichdi-42672r</t>
+  </si>
+  <si>
     <t>7445</t>
   </si>
   <si>
     <t>Minty Couscous</t>
-  </si>
-  <si>
-    <t>Snack/Lunch</t>
-  </si>
-  <si>
-    <t>Veg</t>
   </si>
   <si>
     <t>chopped mint leaves (phudina) ,
@@ -103,9 +314,6 @@
  salt</t>
   </si>
   <si>
-    <t>10 mins</t>
-  </si>
-  <si>
     <t>4 mins</t>
   </si>
   <si>
@@ -133,9 +341,6 @@
   </si>
   <si>
     <t>https://www.tarladalal.com/minty-couscous-7445r</t>
-  </si>
-  <si>
-    <t>Yes</t>
   </si>
   <si>
     <t xml:space="preserve">Yes: 
@@ -200,9 +405,6 @@
   </si>
   <si>
     <t>https://www.tarladalal.com/masala-chawli-3883r</t>
-  </si>
-  <si>
-    <t>Add</t>
   </si>
   <si>
     <t xml:space="preserve">Yes: 
@@ -254,7 +456,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:U9"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -360,25 +562,23 @@
         <v>31</v>
       </c>
       <c r="L2" t="s" s="0">
-        <v>20</v>
-      </c>
-      <c r="M2" s="0"/>
+        <v>32</v>
+      </c>
+      <c r="M2" t="s" s="0">
+        <v>33</v>
+      </c>
       <c r="N2" s="0"/>
-      <c r="O2" t="s" s="0">
-        <v>32</v>
-      </c>
+      <c r="O2" s="0"/>
       <c r="P2" s="0"/>
       <c r="Q2" t="s" s="0">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="R2" t="s" s="0">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="S2" s="0"/>
       <c r="T2" s="0"/>
-      <c r="U2" t="s" s="0">
-        <v>34</v>
-      </c>
+      <c r="U2" s="0"/>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
@@ -388,54 +588,374 @@
         <v>36</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="D3" t="s" s="0">
         <v>24</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="G3" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="H3" t="s" s="0">
         <v>39</v>
       </c>
-      <c r="H3" t="s" s="0">
+      <c r="I3" t="s" s="0">
         <v>40</v>
       </c>
-      <c r="I3" t="s" s="0">
+      <c r="J3" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="K3" t="s" s="0">
         <v>41</v>
       </c>
-      <c r="J3" t="s" s="0">
-        <v>42</v>
-      </c>
-      <c r="K3" t="s" s="0">
-        <v>43</v>
-      </c>
       <c r="L3" t="s" s="0">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="M3" t="s" s="0">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N3" s="0"/>
-      <c r="O3" t="s" s="0">
-        <v>32</v>
-      </c>
+      <c r="O3" s="0"/>
       <c r="P3" s="0"/>
       <c r="Q3" t="s" s="0">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="R3" t="s" s="0">
-        <v>45</v>
-      </c>
-      <c r="S3" t="s" s="0">
-        <v>32</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="S3" s="0"/>
       <c r="T3" s="0"/>
       <c r="U3" s="0"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="G4" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="H4" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="I4" t="s" s="0">
+        <v>47</v>
+      </c>
+      <c r="J4" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="K4" t="s" s="0">
+        <v>49</v>
+      </c>
+      <c r="L4" s="0"/>
+      <c r="M4" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="N4" s="0"/>
+      <c r="O4" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="P4" s="0"/>
+      <c r="Q4" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="R4" s="0"/>
+      <c r="S4" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="T4" s="0"/>
+      <c r="U4" s="0"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="F5" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="G5" t="s" s="0">
+        <v>55</v>
+      </c>
+      <c r="H5" t="s" s="0">
+        <v>56</v>
+      </c>
+      <c r="I5" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="J5" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="K5" t="s" s="0">
+        <v>58</v>
+      </c>
+      <c r="L5" s="0"/>
+      <c r="M5" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="N5" s="0"/>
+      <c r="O5" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="P5" s="0"/>
+      <c r="Q5" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="R5" s="0"/>
+      <c r="S5" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="T5" s="0"/>
+      <c r="U5" s="0"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>59</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="G6" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="H6" t="s" s="0">
+        <v>63</v>
+      </c>
+      <c r="I6" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="J6" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="K6" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="L6" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="M6" s="0"/>
+      <c r="N6" s="0"/>
+      <c r="O6" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="P6" s="0"/>
+      <c r="Q6" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="R6" t="s" s="0">
+        <v>67</v>
+      </c>
+      <c r="S6" s="0"/>
+      <c r="T6" s="0"/>
+      <c r="U6" t="s" s="0">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>69</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="F7" t="s" s="0">
+        <v>72</v>
+      </c>
+      <c r="G7" t="s" s="0">
+        <v>73</v>
+      </c>
+      <c r="H7" t="s" s="0">
+        <v>74</v>
+      </c>
+      <c r="I7" t="s" s="0">
+        <v>75</v>
+      </c>
+      <c r="J7" t="s" s="0">
+        <v>76</v>
+      </c>
+      <c r="K7" t="s" s="0">
+        <v>77</v>
+      </c>
+      <c r="L7" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="M7" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="N7" s="0"/>
+      <c r="O7" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="P7" s="0"/>
+      <c r="Q7" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="R7" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="S7" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="T7" s="0"/>
+      <c r="U7" s="0"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="E8" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="F8" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="G8" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="H8" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="I8" t="s" s="0">
+        <v>47</v>
+      </c>
+      <c r="J8" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="K8" t="s" s="0">
+        <v>49</v>
+      </c>
+      <c r="L8" s="0"/>
+      <c r="M8" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="N8" s="0"/>
+      <c r="O8" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="P8" s="0"/>
+      <c r="Q8" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="R8" s="0"/>
+      <c r="S8" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="T8" s="0"/>
+      <c r="U8" s="0"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="D9" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="E9" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="F9" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="G9" t="s" s="0">
+        <v>55</v>
+      </c>
+      <c r="H9" t="s" s="0">
+        <v>56</v>
+      </c>
+      <c r="I9" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="J9" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="K9" t="s" s="0">
+        <v>58</v>
+      </c>
+      <c r="L9" s="0"/>
+      <c r="M9" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="N9" s="0"/>
+      <c r="O9" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="P9" s="0"/>
+      <c r="Q9" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="R9" s="0"/>
+      <c r="S9" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="T9" s="0"/>
+      <c r="U9" s="0"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -444,7 +964,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:U3"/>
+  <dimension ref="A1:U9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -550,25 +1070,23 @@
         <v>31</v>
       </c>
       <c r="L2" t="s" s="0">
-        <v>20</v>
-      </c>
-      <c r="M2" s="0"/>
+        <v>32</v>
+      </c>
+      <c r="M2" t="s" s="0">
+        <v>33</v>
+      </c>
       <c r="N2" s="0"/>
-      <c r="O2" t="s" s="0">
-        <v>32</v>
-      </c>
+      <c r="O2" s="0"/>
       <c r="P2" s="0"/>
       <c r="Q2" t="s" s="0">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="R2" t="s" s="0">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="S2" s="0"/>
       <c r="T2" s="0"/>
-      <c r="U2" t="s" s="0">
-        <v>34</v>
-      </c>
+      <c r="U2" s="0"/>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
@@ -578,54 +1096,374 @@
         <v>36</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="D3" t="s" s="0">
         <v>24</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="G3" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="H3" t="s" s="0">
         <v>39</v>
       </c>
-      <c r="H3" t="s" s="0">
+      <c r="I3" t="s" s="0">
         <v>40</v>
       </c>
-      <c r="I3" t="s" s="0">
+      <c r="J3" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="K3" t="s" s="0">
         <v>41</v>
       </c>
-      <c r="J3" t="s" s="0">
-        <v>42</v>
-      </c>
-      <c r="K3" t="s" s="0">
-        <v>43</v>
-      </c>
       <c r="L3" t="s" s="0">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="M3" t="s" s="0">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N3" s="0"/>
-      <c r="O3" t="s" s="0">
-        <v>32</v>
-      </c>
+      <c r="O3" s="0"/>
       <c r="P3" s="0"/>
       <c r="Q3" t="s" s="0">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="R3" t="s" s="0">
-        <v>45</v>
-      </c>
-      <c r="S3" t="s" s="0">
-        <v>32</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="S3" s="0"/>
       <c r="T3" s="0"/>
       <c r="U3" s="0"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="G4" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="H4" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="I4" t="s" s="0">
+        <v>47</v>
+      </c>
+      <c r="J4" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="K4" t="s" s="0">
+        <v>49</v>
+      </c>
+      <c r="L4" s="0"/>
+      <c r="M4" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="N4" s="0"/>
+      <c r="O4" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="P4" s="0"/>
+      <c r="Q4" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="R4" s="0"/>
+      <c r="S4" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="T4" s="0"/>
+      <c r="U4" s="0"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="F5" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="G5" t="s" s="0">
+        <v>55</v>
+      </c>
+      <c r="H5" t="s" s="0">
+        <v>56</v>
+      </c>
+      <c r="I5" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="J5" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="K5" t="s" s="0">
+        <v>58</v>
+      </c>
+      <c r="L5" s="0"/>
+      <c r="M5" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="N5" s="0"/>
+      <c r="O5" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="P5" s="0"/>
+      <c r="Q5" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="R5" s="0"/>
+      <c r="S5" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="T5" s="0"/>
+      <c r="U5" s="0"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>59</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="G6" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="H6" t="s" s="0">
+        <v>63</v>
+      </c>
+      <c r="I6" t="s" s="0">
+        <v>64</v>
+      </c>
+      <c r="J6" t="s" s="0">
+        <v>65</v>
+      </c>
+      <c r="K6" t="s" s="0">
+        <v>66</v>
+      </c>
+      <c r="L6" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="M6" s="0"/>
+      <c r="N6" s="0"/>
+      <c r="O6" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="P6" s="0"/>
+      <c r="Q6" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="R6" t="s" s="0">
+        <v>67</v>
+      </c>
+      <c r="S6" s="0"/>
+      <c r="T6" s="0"/>
+      <c r="U6" t="s" s="0">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>69</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="E7" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="F7" t="s" s="0">
+        <v>72</v>
+      </c>
+      <c r="G7" t="s" s="0">
+        <v>73</v>
+      </c>
+      <c r="H7" t="s" s="0">
+        <v>74</v>
+      </c>
+      <c r="I7" t="s" s="0">
+        <v>75</v>
+      </c>
+      <c r="J7" t="s" s="0">
+        <v>76</v>
+      </c>
+      <c r="K7" t="s" s="0">
+        <v>77</v>
+      </c>
+      <c r="L7" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="M7" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="N7" s="0"/>
+      <c r="O7" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="P7" s="0"/>
+      <c r="Q7" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="R7" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="S7" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="T7" s="0"/>
+      <c r="U7" s="0"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>42</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="E8" t="s" s="0">
+        <v>44</v>
+      </c>
+      <c r="F8" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="G8" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="H8" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="I8" t="s" s="0">
+        <v>47</v>
+      </c>
+      <c r="J8" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="K8" t="s" s="0">
+        <v>49</v>
+      </c>
+      <c r="L8" s="0"/>
+      <c r="M8" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="N8" s="0"/>
+      <c r="O8" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="P8" s="0"/>
+      <c r="Q8" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="R8" s="0"/>
+      <c r="S8" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="T8" s="0"/>
+      <c r="U8" s="0"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>50</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>52</v>
+      </c>
+      <c r="D9" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="E9" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="F9" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="G9" t="s" s="0">
+        <v>55</v>
+      </c>
+      <c r="H9" t="s" s="0">
+        <v>56</v>
+      </c>
+      <c r="I9" t="s" s="0">
+        <v>57</v>
+      </c>
+      <c r="J9" t="s" s="0">
+        <v>48</v>
+      </c>
+      <c r="K9" t="s" s="0">
+        <v>58</v>
+      </c>
+      <c r="L9" s="0"/>
+      <c r="M9" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="N9" s="0"/>
+      <c r="O9" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="P9" s="0"/>
+      <c r="Q9" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="R9" s="0"/>
+      <c r="S9" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="T9" s="0"/>
+      <c r="U9" s="0"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -634,7 +1472,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:U2"/>
+  <dimension ref="A1:U4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -707,10 +1545,10 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s" s="0">
         <v>23</v>
@@ -719,48 +1557,154 @@
         <v>24</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="G2" t="s" s="0">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="H2" t="s" s="0">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="I2" t="s" s="0">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="J2" t="s" s="0">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="K2" t="s" s="0">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="L2" t="s" s="0">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="M2" t="s" s="0">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N2" s="0"/>
-      <c r="O2" t="s" s="0">
-        <v>32</v>
-      </c>
+      <c r="O2" s="0"/>
       <c r="P2" s="0"/>
       <c r="Q2" t="s" s="0">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="R2" t="s" s="0">
-        <v>45</v>
-      </c>
-      <c r="S2" t="s" s="0">
-        <v>32</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="S2" s="0"/>
       <c r="T2" s="0"/>
       <c r="U2" s="0"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="C3" t="s" s="0">
+        <v>37</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="E3" t="s" s="0">
+        <v>38</v>
+      </c>
+      <c r="F3" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="G3" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="H3" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="I3" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="J3" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="K3" t="s" s="0">
+        <v>41</v>
+      </c>
+      <c r="L3" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="M3" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="N3" s="0"/>
+      <c r="O3" s="0"/>
+      <c r="P3" s="0"/>
+      <c r="Q3" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="R3" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="S3" s="0"/>
+      <c r="T3" s="0"/>
+      <c r="U3" s="0"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>69</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>70</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>71</v>
+      </c>
+      <c r="F4" t="s" s="0">
+        <v>72</v>
+      </c>
+      <c r="G4" t="s" s="0">
+        <v>73</v>
+      </c>
+      <c r="H4" t="s" s="0">
+        <v>74</v>
+      </c>
+      <c r="I4" t="s" s="0">
+        <v>75</v>
+      </c>
+      <c r="J4" t="s" s="0">
+        <v>76</v>
+      </c>
+      <c r="K4" t="s" s="0">
+        <v>77</v>
+      </c>
+      <c r="L4" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="M4" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="N4" s="0"/>
+      <c r="O4" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="P4" s="0"/>
+      <c r="Q4" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="R4" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="S4" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="T4" s="0"/>
+      <c r="U4" s="0"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -842,10 +1786,10 @@
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>21</v>
+        <v>59</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>22</v>
+        <v>60</v>
       </c>
       <c r="C2" t="s" s="0">
         <v>23</v>
@@ -854,25 +1798,25 @@
         <v>24</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="F2" t="s" s="0">
         <v>26</v>
       </c>
       <c r="G2" t="s" s="0">
-        <v>27</v>
+        <v>62</v>
       </c>
       <c r="H2" t="s" s="0">
-        <v>28</v>
+        <v>63</v>
       </c>
       <c r="I2" t="s" s="0">
-        <v>29</v>
+        <v>64</v>
       </c>
       <c r="J2" t="s" s="0">
-        <v>30</v>
+        <v>65</v>
       </c>
       <c r="K2" t="s" s="0">
-        <v>31</v>
+        <v>66</v>
       </c>
       <c r="L2" t="s" s="0">
         <v>20</v>
@@ -880,19 +1824,19 @@
       <c r="M2" s="0"/>
       <c r="N2" s="0"/>
       <c r="O2" t="s" s="0">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="P2" s="0"/>
       <c r="Q2" t="s" s="0">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="R2" t="s" s="0">
-        <v>33</v>
+        <v>67</v>
       </c>
       <c r="S2" s="0"/>
       <c r="T2" s="0"/>
       <c r="U2" t="s" s="0">
-        <v>34</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>